<commit_message>
amet & assim param search in 1meso
keep track of zoop overconsump, but don't change fish consump
</commit_message>
<xml_diff>
--- a/CODE/Data/Hist_1zoo_1meso_SAUP_comps.xlsx
+++ b/CODE/Data/Hist_1zoo_1meso_SAUP_comps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cpetrik/Dropbox/Princeton/FEISTY/CODE/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720A5F97-1D1A-6E46-988D-2D63517B0BF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0CDEC3A-86D6-8B43-9D57-1D5C8BB928DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="460" windowWidth="31380" windowHeight="16540" xr2:uid="{A0DAAD8F-6CCB-DD45-A7DF-ADFBC6A78C63}"/>
+    <workbookView xWindow="11440" yWindow="460" windowWidth="22640" windowHeight="16540" xr2:uid="{A0DAAD8F-6CCB-DD45-A7DF-ADFBC6A78C63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
   <si>
     <t>Correlations</t>
   </si>
@@ -79,6 +79,15 @@
   </si>
   <si>
     <t>bC=0.3</t>
+  </si>
+  <si>
+    <t>2 zoo</t>
+  </si>
+  <si>
+    <t>2zoo</t>
+  </si>
+  <si>
+    <t>Combo</t>
   </si>
 </sst>
 </file>
@@ -434,144 +443,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBF2C46F-477B-3B45-A132-A4B65918AE83}">
-  <dimension ref="A1:U9"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>15</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>17</v>
       </c>
-      <c r="M2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N2" t="s">
-        <v>9</v>
-      </c>
-      <c r="O2" t="s">
-        <v>10</v>
-      </c>
-      <c r="P2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>13</v>
-      </c>
-      <c r="R2" t="s">
-        <v>14</v>
-      </c>
-      <c r="S2" t="s">
-        <v>16</v>
-      </c>
-      <c r="T2" t="s">
-        <v>15</v>
-      </c>
-      <c r="U2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="L2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.14000000000000001</v>
+        <v>0.21</v>
       </c>
       <c r="C3">
         <v>0.14000000000000001</v>
       </c>
       <c r="D3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E3">
         <v>0.11</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>0.18</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.09</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>0.08</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>0.12</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>0.19</v>
       </c>
-      <c r="L3" t="s">
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>1.59</v>
-      </c>
-      <c r="N3">
-        <v>1.59</v>
-      </c>
-      <c r="O3">
-        <v>1.67</v>
-      </c>
-      <c r="P3">
-        <v>1.75</v>
-      </c>
-      <c r="Q3">
-        <v>1.67</v>
-      </c>
-      <c r="R3">
-        <v>1.68</v>
-      </c>
-      <c r="S3">
-        <v>1.71</v>
-      </c>
-      <c r="T3">
-        <v>1.83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="K3">
+        <v>0.27</v>
+      </c>
+      <c r="L3">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.36</v>
+        <v>0.41</v>
       </c>
       <c r="C4">
         <v>0.36</v>
@@ -580,336 +553,540 @@
         <v>0.36</v>
       </c>
       <c r="E4">
+        <v>0.36</v>
+      </c>
+      <c r="F4">
         <v>0.32</v>
-      </c>
-      <c r="F4">
-        <v>0.34</v>
       </c>
       <c r="G4">
         <v>0.34</v>
       </c>
       <c r="H4">
+        <v>0.34</v>
+      </c>
+      <c r="I4">
         <v>0.36</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>0.26</v>
       </c>
-      <c r="L4" t="s">
-        <v>2</v>
-      </c>
-      <c r="M4">
-        <v>3.17</v>
-      </c>
-      <c r="N4">
-        <v>3.17</v>
-      </c>
-      <c r="O4">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="P4">
-        <v>0.93</v>
-      </c>
-      <c r="Q4">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="R4">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="S4" s="2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="T4">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="K4">
+        <v>0.23</v>
+      </c>
+      <c r="L4">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.57999999999999996</v>
+        <v>0.59</v>
       </c>
       <c r="C5">
         <v>0.57999999999999996</v>
       </c>
       <c r="D5">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E5">
         <v>0.59</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>0.56000000000000005</v>
-      </c>
-      <c r="F5">
-        <v>0.59</v>
       </c>
       <c r="G5">
         <v>0.59</v>
       </c>
       <c r="H5">
+        <v>0.59</v>
+      </c>
+      <c r="I5">
         <v>0.57999999999999996</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>0.56000000000000005</v>
       </c>
-      <c r="L5" t="s">
-        <v>3</v>
-      </c>
-      <c r="M5">
-        <v>0.45</v>
-      </c>
-      <c r="N5">
-        <v>0.45</v>
-      </c>
-      <c r="O5">
-        <v>0.45</v>
-      </c>
-      <c r="P5">
-        <v>0.47</v>
-      </c>
-      <c r="Q5">
-        <v>0.45</v>
-      </c>
-      <c r="R5">
-        <v>0.46</v>
-      </c>
-      <c r="S5">
-        <v>0.46</v>
-      </c>
-      <c r="T5">
-        <v>0.46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="K5">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="L5">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.33</v>
+        <v>0.34</v>
       </c>
       <c r="C6">
         <v>0.33</v>
       </c>
       <c r="D6">
+        <v>0.33</v>
+      </c>
+      <c r="E6">
         <v>0.36</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>0.32</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <v>0.36</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>0.4</v>
       </c>
-      <c r="H6" s="2">
+      <c r="I6" s="2">
         <v>0.39</v>
       </c>
-      <c r="I6" s="2">
+      <c r="J6" s="2">
         <v>0.32</v>
       </c>
-      <c r="J6" s="2"/>
-      <c r="L6" t="s">
-        <v>4</v>
-      </c>
-      <c r="M6">
-        <v>0.45</v>
-      </c>
-      <c r="N6">
-        <v>0.45</v>
-      </c>
-      <c r="O6">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="P6">
-        <v>0.48</v>
-      </c>
-      <c r="Q6">
-        <v>0.54</v>
-      </c>
-      <c r="R6">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="S6">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="T6">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="K6" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
-        <v>0.67896416568119</v>
+      <c r="B7">
+        <v>0.61</v>
       </c>
       <c r="C7" s="2">
         <v>0.67896416568119</v>
       </c>
       <c r="D7" s="2">
+        <v>0.67896416568119</v>
+      </c>
+      <c r="E7" s="2">
         <v>0.66561376764047897</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <v>0.60620599510836504</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G7" s="2">
         <v>0.67209697708201699</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7" s="2">
         <v>0.70236371776633699</v>
       </c>
-      <c r="H7" s="2">
+      <c r="I7" s="2">
         <v>0.68389331789813501</v>
       </c>
-      <c r="I7" s="2">
+      <c r="J7" s="2">
         <v>0.52669211222152201</v>
       </c>
-      <c r="J7" s="2"/>
-      <c r="L7" t="s">
-        <v>5</v>
-      </c>
-      <c r="M7" s="2">
-        <v>0.26260070035359201</v>
-      </c>
-      <c r="N7" s="2">
-        <v>0.26260070035359201</v>
-      </c>
-      <c r="O7" s="2">
-        <v>0.48789085356416001</v>
-      </c>
-      <c r="P7" s="2">
-        <v>0.387426074307402</v>
-      </c>
-      <c r="Q7" s="2">
-        <v>0.48103885301796001</v>
-      </c>
-      <c r="R7" s="2">
-        <v>0.40893734951537902</v>
-      </c>
-      <c r="S7" s="2">
-        <v>0.398845330715841</v>
-      </c>
-      <c r="T7" s="2">
-        <v>0.321805015988259</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="K7" s="2">
+        <v>0.16285527723332799</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0.24524566909832299</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2">
-        <v>0.61718342150935002</v>
+      <c r="B8">
+        <v>0.61</v>
       </c>
       <c r="C8" s="2">
         <v>0.61718342150935002</v>
       </c>
       <c r="D8" s="2">
+        <v>0.61718342150935002</v>
+      </c>
+      <c r="E8" s="2">
         <v>0.60330322720340501</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <v>0.51003346363533597</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8" s="2">
         <v>0.61150850562663495</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <v>0.63850297028020098</v>
       </c>
-      <c r="H8" s="2">
+      <c r="I8" s="2">
         <v>0.60774437314741903</v>
       </c>
-      <c r="I8" s="2">
+      <c r="J8" s="2">
         <v>0.385727909198399</v>
       </c>
-      <c r="J8" s="2"/>
-      <c r="L8" t="s">
-        <v>6</v>
-      </c>
-      <c r="M8" s="2">
-        <v>0.29508377350571302</v>
-      </c>
-      <c r="N8" s="2">
-        <v>0.29508377350571302</v>
-      </c>
-      <c r="O8" s="2">
-        <v>0.51630691823602104</v>
-      </c>
-      <c r="P8" s="2">
-        <v>0.42306817823831</v>
-      </c>
-      <c r="Q8" s="2">
-        <v>0.50993474374470105</v>
-      </c>
-      <c r="R8" s="2">
-        <v>0.44114020712785201</v>
-      </c>
-      <c r="S8" s="2">
-        <v>0.43335592968410602</v>
-      </c>
-      <c r="T8" s="2">
-        <v>0.35697022485230201</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="K8" s="2">
+        <v>3.7496384493445702E-2</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0.12721411976222999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="2">
-        <v>0.359494849707093</v>
+        <v>0.3</v>
       </c>
       <c r="C9" s="2">
         <v>0.359494849707093</v>
       </c>
       <c r="D9" s="2">
+        <v>0.359494849707093</v>
+      </c>
+      <c r="E9" s="2">
         <v>0.28202787961935799</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="2">
         <v>0.14589739243920699</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G9" s="2">
         <v>0.27669521729354102</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H9" s="2">
         <v>0.27631871875057501</v>
       </c>
-      <c r="H9" s="2">
+      <c r="I9" s="2">
         <v>0.26351175445218</v>
       </c>
-      <c r="I9" s="2">
+      <c r="J9" s="2">
         <v>3.9194588760408898E-2</v>
       </c>
-      <c r="J9" s="2"/>
-      <c r="L9" t="s">
+      <c r="K9" s="2">
+        <v>-0.27816507325916401</v>
+      </c>
+      <c r="L9" s="2">
+        <v>-0.20053309153743501</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" t="s">
+        <v>16</v>
+      </c>
+      <c r="J14" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" t="s">
+        <v>17</v>
+      </c>
+      <c r="L14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>1.44</v>
+      </c>
+      <c r="C15">
+        <v>1.59</v>
+      </c>
+      <c r="D15">
+        <v>1.59</v>
+      </c>
+      <c r="E15">
+        <v>1.67</v>
+      </c>
+      <c r="F15">
+        <v>1.75</v>
+      </c>
+      <c r="G15">
+        <v>1.67</v>
+      </c>
+      <c r="H15">
+        <v>1.68</v>
+      </c>
+      <c r="I15">
+        <v>1.71</v>
+      </c>
+      <c r="J15">
+        <v>1.83</v>
+      </c>
+      <c r="K15">
+        <v>2.16</v>
+      </c>
+      <c r="L15">
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>1.73</v>
+      </c>
+      <c r="C16">
+        <v>3.17</v>
+      </c>
+      <c r="D16">
+        <v>3.17</v>
+      </c>
+      <c r="E16">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="F16">
+        <v>0.93</v>
+      </c>
+      <c r="G16">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="H16">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="I16" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J16">
+        <v>0.98</v>
+      </c>
+      <c r="K16">
+        <v>1.21</v>
+      </c>
+      <c r="L16">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>0.45</v>
+      </c>
+      <c r="C17">
+        <v>0.45</v>
+      </c>
+      <c r="D17">
+        <v>0.45</v>
+      </c>
+      <c r="E17">
+        <v>0.45</v>
+      </c>
+      <c r="F17">
+        <v>0.47</v>
+      </c>
+      <c r="G17">
+        <v>0.45</v>
+      </c>
+      <c r="H17">
+        <v>0.46</v>
+      </c>
+      <c r="I17">
+        <v>0.46</v>
+      </c>
+      <c r="J17">
+        <v>0.46</v>
+      </c>
+      <c r="K17">
+        <v>0.47</v>
+      </c>
+      <c r="L17">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="C18">
+        <v>0.45</v>
+      </c>
+      <c r="D18">
+        <v>0.45</v>
+      </c>
+      <c r="E18">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F18">
+        <v>0.48</v>
+      </c>
+      <c r="G18">
+        <v>0.54</v>
+      </c>
+      <c r="H18">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="I18">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="J18">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K18">
+        <v>0.74</v>
+      </c>
+      <c r="L18">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.26260070035359201</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.26260070035359201</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.48789085356416001</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.387426074307402</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0.48103885301796001</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0.40893734951537902</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0.398845330715841</v>
+      </c>
+      <c r="J19" s="2">
+        <v>0.321805015988259</v>
+      </c>
+      <c r="K19" s="2">
+        <v>0.33115544118483797</v>
+      </c>
+      <c r="L19" s="2">
+        <v>0.27947499964217698</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.29508377350571302</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.29508377350571302</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.51630691823602104</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.42306817823831</v>
+      </c>
+      <c r="G20" s="2">
+        <v>0.50993474374470105</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0.44114020712785201</v>
+      </c>
+      <c r="I20" s="2">
+        <v>0.43335592968410602</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0.35697022485230201</v>
+      </c>
+      <c r="K20" s="2">
+        <v>0.36183006303620902</v>
+      </c>
+      <c r="L20" s="2">
+        <v>0.30240560604393102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>7</v>
       </c>
-      <c r="M9" s="2">
+      <c r="B21" s="2">
+        <v>0.33</v>
+      </c>
+      <c r="C21" s="2">
         <v>0.32694000354191199</v>
       </c>
-      <c r="N9" s="2">
+      <c r="D21" s="2">
         <v>0.32694000354191199</v>
       </c>
-      <c r="O9" s="2">
+      <c r="E21" s="2">
         <v>0.47707396821102199</v>
       </c>
-      <c r="P9" s="2">
+      <c r="F21" s="2">
         <v>0.42040639404340102</v>
       </c>
-      <c r="Q9" s="2">
+      <c r="G21" s="2">
         <v>0.47431171204765499</v>
       </c>
-      <c r="R9" s="2">
+      <c r="H21" s="2">
         <v>0.42254026413189699</v>
       </c>
-      <c r="S9" s="2">
+      <c r="I21" s="2">
         <v>0.41754704982104501</v>
       </c>
-      <c r="T9" s="2">
+      <c r="J21" s="2">
         <v>0.38406761182306398</v>
+      </c>
+      <c r="K21" s="2">
+        <v>0.42899133261612798</v>
+      </c>
+      <c r="L21" s="2">
+        <v>0.39545814302441901</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="B1:L1"/>
+    <mergeCell ref="B13:L13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>